<commit_message>
TagBuilder Update: Version of Deisy with Marionette
</commit_message>
<xml_diff>
--- a/resources/formats/TaggingRequest_2021.xlsx
+++ b/resources/formats/TaggingRequest_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryoma\TagBuilder\resources\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xaxis\tagCalc\tagModules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB050B-7A96-49FD-AE6F-4ACCB796AABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABCE2EF-7A8F-426A-A0DE-864AB70F0945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
   <si>
     <t>Agencia</t>
   </si>
@@ -324,9 +324,6 @@
   </si>
   <si>
     <t>u/p</t>
-  </si>
-  <si>
-    <t>Microconvertion</t>
   </si>
 </sst>
 </file>
@@ -690,22 +687,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,18 +697,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,1050 +1543,1050 @@
   </cols>
   <sheetData>
     <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
       <c r="H71" s="2"/>
     </row>
     <row r="72" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
       <c r="H73" s="2"/>
     </row>
     <row r="74" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="25"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="25"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="25"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="25"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="25"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="2"/>
     </row>
     <row r="90" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="25"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="25"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="25"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="25"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
       <c r="H98" s="2"/>
     </row>
     <row r="99" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="25"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
       <c r="H99" s="2"/>
     </row>
     <row r="100" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
       <c r="H100" s="2"/>
     </row>
     <row r="101" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23"/>
       <c r="H101" s="2"/>
     </row>
     <row r="102" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
+      <c r="B102" s="23"/>
+      <c r="C102" s="23"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="23"/>
       <c r="H102" s="2"/>
     </row>
     <row r="103" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="25"/>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="23"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="23"/>
       <c r="H103" s="2"/>
     </row>
     <row r="104" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="25"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
+      <c r="B104" s="23"/>
+      <c r="C104" s="23"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
       <c r="H104" s="2"/>
     </row>
     <row r="105" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="25"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="23"/>
       <c r="H105" s="2"/>
     </row>
     <row r="106" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="25"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="25"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
       <c r="H106" s="2"/>
     </row>
     <row r="107" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="25"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="25"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="23"/>
       <c r="H107" s="2"/>
     </row>
     <row r="108" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="25"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="25"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="23"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23"/>
       <c r="H108" s="2"/>
     </row>
     <row r="109" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
       <c r="H109" s="2"/>
     </row>
     <row r="110" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="25"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
       <c r="H110" s="2"/>
     </row>
     <row r="111" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="25"/>
-      <c r="G111" s="25"/>
+      <c r="B111" s="23"/>
+      <c r="C111" s="23"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="23"/>
       <c r="H111" s="2"/>
     </row>
     <row r="112" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="25"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
       <c r="H112" s="2"/>
     </row>
     <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="25"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="25"/>
-      <c r="G113" s="25"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23"/>
     </row>
     <row r="114" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
-      <c r="G114" s="25"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
     </row>
     <row r="115" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="25"/>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="25"/>
-      <c r="G115" s="25"/>
+      <c r="B115" s="23"/>
+      <c r="C115" s="23"/>
+      <c r="D115" s="23"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="23"/>
+      <c r="G115" s="23"/>
     </row>
     <row r="116" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="25"/>
-      <c r="C116" s="25"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="25"/>
-      <c r="G116" s="25"/>
+      <c r="B116" s="23"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="23"/>
+      <c r="G116" s="23"/>
     </row>
     <row r="117" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="25"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="25"/>
-      <c r="G117" s="25"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="23"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="23"/>
     </row>
     <row r="118" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="25"/>
-      <c r="C118" s="25"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="25"/>
-      <c r="G118" s="25"/>
+      <c r="B118" s="23"/>
+      <c r="C118" s="23"/>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23"/>
     </row>
     <row r="119" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="25"/>
-      <c r="C119" s="25"/>
-      <c r="D119" s="25"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="25"/>
-      <c r="G119" s="25"/>
+      <c r="B119" s="23"/>
+      <c r="C119" s="23"/>
+      <c r="D119" s="23"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="23"/>
+      <c r="G119" s="23"/>
     </row>
     <row r="120" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="25"/>
-      <c r="C120" s="25"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="25"/>
-      <c r="F120" s="25"/>
-      <c r="G120" s="25"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="23"/>
     </row>
     <row r="121" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
-      <c r="G121" s="25"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="23"/>
     </row>
     <row r="122" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="25"/>
-      <c r="C122" s="25"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="25"/>
-      <c r="G122" s="25"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="23"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="23"/>
     </row>
     <row r="123" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="25"/>
-      <c r="C123" s="25"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="25"/>
-      <c r="G123" s="25"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="23"/>
     </row>
     <row r="124" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="25"/>
-      <c r="G124" s="25"/>
+      <c r="B124" s="23"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="23"/>
     </row>
     <row r="125" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="25"/>
-      <c r="C125" s="25"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="25"/>
-      <c r="G125" s="25"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="23"/>
+      <c r="G125" s="23"/>
     </row>
     <row r="126" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="25"/>
-      <c r="C126" s="25"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="25"/>
-      <c r="G126" s="25"/>
+      <c r="B126" s="23"/>
+      <c r="C126" s="23"/>
+      <c r="D126" s="23"/>
+      <c r="E126" s="23"/>
+      <c r="F126" s="23"/>
+      <c r="G126" s="23"/>
     </row>
     <row r="127" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="25"/>
-      <c r="C127" s="25"/>
-      <c r="D127" s="25"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="25"/>
-      <c r="G127" s="25"/>
+      <c r="B127" s="23"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="23"/>
+      <c r="E127" s="23"/>
+      <c r="F127" s="23"/>
+      <c r="G127" s="23"/>
     </row>
     <row r="128" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
-      <c r="G128" s="25"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="23"/>
     </row>
     <row r="129" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="25"/>
-      <c r="C129" s="25"/>
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="25"/>
-      <c r="G129" s="25"/>
+      <c r="B129" s="23"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="23"/>
+      <c r="F129" s="23"/>
+      <c r="G129" s="23"/>
     </row>
     <row r="130" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
-      <c r="D130" s="25"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="25"/>
-      <c r="G130" s="25"/>
+      <c r="B130" s="23"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="23"/>
     </row>
     <row r="131" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="25"/>
-      <c r="C131" s="25"/>
-      <c r="D131" s="25"/>
-      <c r="E131" s="25"/>
-      <c r="F131" s="25"/>
-      <c r="G131" s="25"/>
+      <c r="B131" s="23"/>
+      <c r="C131" s="23"/>
+      <c r="D131" s="23"/>
+      <c r="E131" s="23"/>
+      <c r="F131" s="23"/>
+      <c r="G131" s="23"/>
     </row>
     <row r="132" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="25"/>
-      <c r="C132" s="25"/>
-      <c r="D132" s="25"/>
-      <c r="E132" s="25"/>
-      <c r="F132" s="25"/>
-      <c r="G132" s="25"/>
+      <c r="B132" s="23"/>
+      <c r="C132" s="23"/>
+      <c r="D132" s="23"/>
+      <c r="E132" s="23"/>
+      <c r="F132" s="23"/>
+      <c r="G132" s="23"/>
     </row>
     <row r="133" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="25"/>
-      <c r="C133" s="25"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="25"/>
-      <c r="F133" s="25"/>
-      <c r="G133" s="25"/>
+      <c r="B133" s="23"/>
+      <c r="C133" s="23"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="23"/>
+      <c r="F133" s="23"/>
+      <c r="G133" s="23"/>
     </row>
     <row r="134" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="25"/>
-      <c r="C134" s="25"/>
-      <c r="D134" s="25"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="25"/>
-      <c r="G134" s="25"/>
+      <c r="B134" s="23"/>
+      <c r="C134" s="23"/>
+      <c r="D134" s="23"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="23"/>
     </row>
     <row r="135" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="25"/>
-      <c r="C135" s="25"/>
-      <c r="D135" s="25"/>
-      <c r="E135" s="25"/>
-      <c r="F135" s="25"/>
-      <c r="G135" s="25"/>
+      <c r="B135" s="23"/>
+      <c r="C135" s="23"/>
+      <c r="D135" s="23"/>
+      <c r="E135" s="23"/>
+      <c r="F135" s="23"/>
+      <c r="G135" s="23"/>
     </row>
     <row r="136" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="25"/>
-      <c r="C136" s="25"/>
-      <c r="D136" s="25"/>
-      <c r="E136" s="25"/>
-      <c r="F136" s="25"/>
-      <c r="G136" s="25"/>
+      <c r="B136" s="23"/>
+      <c r="C136" s="23"/>
+      <c r="D136" s="23"/>
+      <c r="E136" s="23"/>
+      <c r="F136" s="23"/>
+      <c r="G136" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2652,7 +2649,7 @@
       <c r="T2" s="10"/>
     </row>
     <row r="3" spans="2:20" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -2669,7 +2666,7 @@
       </c>
     </row>
     <row r="4" spans="2:20" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="36" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -2686,7 +2683,7 @@
       </c>
     </row>
     <row r="5" spans="2:20" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -2695,7 +2692,7 @@
       <c r="D5" s="22"/>
     </row>
     <row r="6" spans="2:20" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4369,8 +4366,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A11:AMH303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4476,57 +4473,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="25"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="24"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -4544,7 +4541,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="4"/>
@@ -4561,7 +4558,7 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -4576,7 +4573,7 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="4"/>
@@ -4593,7 +4590,7 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="27"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -4608,8 +4605,8 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="26" t="s">
-        <v>51</v>
+      <c r="B35" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -4625,7 +4622,7 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -4910,6 +4907,11 @@
     <row r="303" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J28:K28"/>
@@ -4919,11 +4921,6 @@
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="I29:I30"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G36" xr:uid="{159AEBD0-1FCE-4A68-92F1-36C3B0B6D6AE}">
@@ -5054,57 +5051,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="25"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="24"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -5122,7 +5119,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="4"/>
@@ -5139,7 +5136,7 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -5154,7 +5151,7 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="33"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -5169,7 +5166,7 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="4"/>
@@ -5186,7 +5183,7 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="27"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -5201,7 +5198,7 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -5216,7 +5213,7 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="27"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -5231,7 +5228,7 @@
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="27"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -5246,7 +5243,7 @@
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="27" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="4"/>
@@ -5263,7 +5260,7 @@
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="27"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -5278,7 +5275,7 @@
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="27"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -5293,7 +5290,7 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="32"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -5308,7 +5305,7 @@
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="32"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -5737,57 +5734,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="25"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="24"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -5805,276 +5802,276 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
     </row>
     <row r="33" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="34"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="34"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="34"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
     </row>
     <row r="37" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="34"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
     </row>
     <row r="38" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="34"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
     </row>
     <row r="39" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="34"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
     </row>
     <row r="40" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="34"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
     </row>
     <row r="41" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="34"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
     </row>
     <row r="42" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="34"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
     </row>
     <row r="43" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="34"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="36"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
     </row>
     <row r="44" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="34"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="36"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="33"/>
     </row>
     <row r="45" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="34"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="36"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
     </row>
     <row r="46" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="34"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="36"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="33"/>
     </row>
     <row r="47" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="34"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="36"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
     </row>
     <row r="48" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="34"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="34"/>
     </row>
     <row r="49" spans="6:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F49" s="8"/>
@@ -6347,6 +6344,17 @@
     <row r="315" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B31:B48"/>
+    <mergeCell ref="C31:C48"/>
+    <mergeCell ref="D31:D48"/>
+    <mergeCell ref="E31:E48"/>
+    <mergeCell ref="G31:G48"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="L31:L48"/>
     <mergeCell ref="M31:M48"/>
     <mergeCell ref="N31:N48"/>
@@ -6359,17 +6367,6 @@
     <mergeCell ref="J31:J48"/>
     <mergeCell ref="K31:K48"/>
     <mergeCell ref="H31:H48"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B31:B48"/>
-    <mergeCell ref="C31:C48"/>
-    <mergeCell ref="D31:D48"/>
-    <mergeCell ref="E31:E48"/>
-    <mergeCell ref="G31:G48"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C48" xr:uid="{313610C3-1725-4BDE-B2FF-49FB559662B0}">

</xml_diff>

<commit_message>
TagBuilder Update: Revision of Taboola Platform.
</commit_message>
<xml_diff>
--- a/resources/formats/TaggingRequest_2021.xlsx
+++ b/resources/formats/TaggingRequest_2021.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryoma\TagBuilder\resources\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CB050B-7A96-49FD-AE6F-4ACCB796AABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D749A92-2A2B-462B-8733-5EC7F6F8E4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Tagging Request " sheetId="1" r:id="rId1"/>
-    <sheet name="Listas" sheetId="8" state="hidden" r:id="rId2"/>
+    <sheet name="Listas" sheetId="8" r:id="rId2"/>
     <sheet name="Tagging Request" sheetId="2" r:id="rId3"/>
     <sheet name="Funnel" sheetId="7" r:id="rId4"/>
     <sheet name="Sections" sheetId="4" r:id="rId5"/>
@@ -697,15 +697,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,18 +706,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2605,7 +2605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C476D17-5786-4464-A0F3-8A2E9CCCA677}">
   <dimension ref="A1:CD559"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4369,7 +4369,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A11:AMH303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -4476,57 +4476,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="27"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="26"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -4544,7 +4544,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="29" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="4"/>
@@ -4561,7 +4561,7 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -4576,7 +4576,7 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="4"/>
@@ -4593,7 +4593,7 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="27"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -4608,7 +4608,7 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C35" s="4"/>
@@ -4625,7 +4625,7 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -4910,6 +4910,11 @@
     <row r="303" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J28:K28"/>
@@ -4919,11 +4924,6 @@
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="I29:I30"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G36" xr:uid="{159AEBD0-1FCE-4A68-92F1-36C3B0B6D6AE}">
@@ -5054,57 +5054,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="27"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="26"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -5122,7 +5122,7 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="29" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="4"/>
@@ -5139,7 +5139,7 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -5169,7 +5169,7 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="4"/>
@@ -5186,7 +5186,7 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="27"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -5201,7 +5201,7 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -5216,7 +5216,7 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="27"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -5231,7 +5231,7 @@
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="27"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -5246,7 +5246,7 @@
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="4"/>
@@ -5263,7 +5263,7 @@
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="27"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -5278,7 +5278,7 @@
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="27"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -5293,7 +5293,7 @@
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="32"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -5308,7 +5308,7 @@
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="32"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -5737,57 +5737,57 @@
     </row>
     <row r="27" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="31"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="30"/>
+      <c r="K29" s="27"/>
       <c r="L29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="29"/>
+      <c r="N29" s="26"/>
     </row>
     <row r="30" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
       <c r="J30" s="3" t="s">
         <v>28</v>
       </c>
@@ -5805,276 +5805,276 @@
       </c>
     </row>
     <row r="31" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
     </row>
     <row r="32" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
     </row>
     <row r="33" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="34"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
     </row>
     <row r="34" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
     </row>
     <row r="35" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="34"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
     </row>
     <row r="36" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="34"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
     </row>
     <row r="37" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="34"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
     </row>
     <row r="38" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="34"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
     </row>
     <row r="39" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="34"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
     </row>
     <row r="40" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="34"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
     </row>
     <row r="41" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="34"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
     </row>
     <row r="42" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="34"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
     </row>
     <row r="43" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="34"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="36"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
     </row>
     <row r="44" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="34"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="36"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
     </row>
     <row r="45" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="34"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="36"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
     </row>
     <row r="46" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="34"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="36"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
     </row>
     <row r="47" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="34"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="36"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
     </row>
     <row r="48" spans="2:14" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="34"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
     </row>
     <row r="49" spans="6:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F49" s="8"/>
@@ -6347,6 +6347,17 @@
     <row r="315" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B31:B48"/>
+    <mergeCell ref="C31:C48"/>
+    <mergeCell ref="D31:D48"/>
+    <mergeCell ref="E31:E48"/>
+    <mergeCell ref="G31:G48"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="L31:L48"/>
     <mergeCell ref="M31:M48"/>
     <mergeCell ref="N31:N48"/>
@@ -6359,17 +6370,6 @@
     <mergeCell ref="J31:J48"/>
     <mergeCell ref="K31:K48"/>
     <mergeCell ref="H31:H48"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B31:B48"/>
-    <mergeCell ref="C31:C48"/>
-    <mergeCell ref="D31:D48"/>
-    <mergeCell ref="E31:E48"/>
-    <mergeCell ref="G31:G48"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C48" xr:uid="{313610C3-1725-4BDE-B2FF-49FB559662B0}">

</xml_diff>

<commit_message>
TagBuilder Update: Tags and Triggers Btn type in Measurement Strategy.
</commit_message>
<xml_diff>
--- a/resources/formats/TaggingRequest_2021.xlsx
+++ b/resources/formats/TaggingRequest_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryoma\TagBuilder\resources\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821BD197-E9A7-4E19-9246-99340D203438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5998C155-A09B-439E-810D-10FAE01119A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4511,7 +4511,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AMH356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TagBuilder Update: GA4 Integration Beta version.
</commit_message>
<xml_diff>
--- a/resources/formats/TaggingRequest_2021.xlsx
+++ b/resources/formats/TaggingRequest_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryoma\TagBuilder\resources\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5998C155-A09B-439E-810D-10FAE01119A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2562A9C0-E361-4EA5-84CB-6B500DC4F7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Agencia</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Taboola - Twitter - TikTok</t>
+  </si>
+  <si>
+    <t>GA4  ID</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -852,6 +855,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1648,7 +1660,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A18:AMJ136"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:G136"/>
     </sheetView>
   </sheetViews>
@@ -4511,8 +4523,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AMH356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4587,7 +4599,7 @@
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="1"/>
       <c r="G11" s="1"/>
     </row>
@@ -4595,7 +4607,7 @@
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -4603,12 +4615,12 @@
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="1"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="1"/>
       <c r="G14" s="1"/>
     </row>
@@ -4616,7 +4628,7 @@
       <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="1"/>
       <c r="G15" s="1"/>
     </row>
@@ -4624,7 +4636,7 @@
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="46" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1"/>
@@ -4634,7 +4646,7 @@
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="46" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="1"/>
@@ -4644,7 +4656,7 @@
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="46" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="1"/>
@@ -4654,7 +4666,7 @@
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="1"/>
@@ -4664,7 +4676,7 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="46" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="1"/>
@@ -4674,7 +4686,7 @@
       <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="1"/>
       <c r="G21" s="1"/>
     </row>
@@ -4682,20 +4694,23 @@
       <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
+      <c r="B24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="48"/>
       <c r="D24" s="1"/>
       <c r="G24" s="1"/>
     </row>
@@ -8515,8 +8530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8E1451-794D-4AAA-996A-CBECC3B02661}">
   <dimension ref="A11:AMH44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8614,10 +8629,16 @@
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="2:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="27" spans="2:14" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8928,8 +8949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704531C-E89D-482F-A691-8949287AF91E}">
   <dimension ref="A11:AMH49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9031,6 +9052,12 @@
         <v>16</v>
       </c>
       <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="2:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="27" spans="2:14" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="2:14" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>